<commit_message>
first draft done! added funding_server module with new look functionalities
</commit_message>
<xml_diff>
--- a/data/Apple_AF_Steinfurt_wRisk_30.xlsx
+++ b/data/Apple_AF_Steinfurt_wRisk_30.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\data\Apple_Agroforestry_System\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\Project_report\Deliverables\D4.3_Model_Comparison\Apple_Agroforestry\Apple_Agroforestry\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3496591E-EC13-4077-8E3E-BEB4F6A6CA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193E747E-D065-4396-9BDD-DCBD4EBFDC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="2" r:id="rId1"/>
@@ -21,14 +21,13 @@
     <sheet name="Sheet5" sheetId="8" r:id="rId6"/>
     <sheet name="Sheet6" sheetId="10" r:id="rId7"/>
     <sheet name="Sheet7" sheetId="11" r:id="rId8"/>
-    <sheet name="Sheet8" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="299">
   <si>
     <t>variable</t>
   </si>
@@ -450,12 +449,6 @@
     <t>person-chalkboard</t>
   </si>
   <si>
-    <t>Funding (from external sources)</t>
-  </si>
-  <si>
-    <t>check-double</t>
-  </si>
-  <si>
     <t>square-poll-vertical</t>
   </si>
   <si>
@@ -921,58 +914,16 @@
     <t>Size of the arable field [ha]</t>
   </si>
   <si>
-    <t>Data analyst; Agroforestry farming</t>
-  </si>
-  <si>
     <t>Risks</t>
   </si>
   <si>
     <t>Crop Coefficients</t>
   </si>
   <si>
-    <t>AF1_total_annual_funding_c</t>
-  </si>
-  <si>
-    <t>Maintenance support</t>
-  </si>
-  <si>
-    <t>Annual maintenance support: Lump sum of funds received annually from external sources in order to maintain the agroforestry system [€]</t>
-  </si>
-  <si>
-    <t>Policy analysis;Agroforestry farming</t>
-  </si>
-  <si>
-    <t>selected_percentage_c</t>
-  </si>
-  <si>
-    <t>unitless</t>
-  </si>
-  <si>
-    <t>Establishment support as a percentage of total investment costs?</t>
-  </si>
-  <si>
-    <t>Shall "Percentage investment funded" be applied?</t>
-  </si>
-  <si>
-    <t>AF1_percentage_values_c</t>
-  </si>
-  <si>
-    <t>ratio</t>
-  </si>
-  <si>
-    <t>Establishment support (as a percentage of total investment costs)</t>
-  </si>
-  <si>
-    <t>Percentage investment funded: Funds received only once from external sources, as a proportion of the investment cost [ratio]</t>
-  </si>
-  <si>
-    <t>AF1_total_one_time_funding_c</t>
-  </si>
-  <si>
-    <t>Establishment support (independent of total investment costs)</t>
-  </si>
-  <si>
-    <t>Establishment funding support: Lump sum of funds received only once from external sources, regardless of the investment costs [€]</t>
+    <t>Data analyst;Agroforestry farming</t>
+  </si>
+  <si>
+    <t>tnorm_0_1</t>
   </si>
 </sst>
 </file>
@@ -1322,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19247B9C-F4A5-4DCC-BF21-E18D3CC8C8F5}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1384,26 +1335,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B8" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B9" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1416,12 +1359,13 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1438,25 +1382,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1473,19 +1417,19 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I2">
         <v>1000</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1502,16 +1446,16 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1534,19 +1478,19 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1563,24 +1507,24 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B6" s="1">
         <v>1000</v>
@@ -1592,22 +1536,22 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" t="s">
         <v>150</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>151</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
         <v>152</v>
-      </c>
-      <c r="H6" t="s">
-        <v>153</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1642,25 +1586,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1677,19 +1621,19 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I2">
         <v>0.1</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1706,16 +1650,16 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1732,16 +1676,16 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1758,19 +1702,19 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I5">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1787,19 +1731,19 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I6">
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1816,19 +1760,19 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I7">
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1845,19 +1789,19 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
+        <v>238</v>
+      </c>
+      <c r="F8" t="s">
         <v>240</v>
       </c>
-      <c r="F8" t="s">
-        <v>242</v>
-      </c>
       <c r="H8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1874,19 +1818,19 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1903,19 +1847,19 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1932,19 +1876,19 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I11">
         <v>0.1</v>
       </c>
       <c r="J11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1961,19 +1905,19 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I12">
         <v>100</v>
       </c>
       <c r="J12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1990,19 +1934,19 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2019,19 +1963,19 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2048,19 +1992,19 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F15" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I15">
         <v>0.1</v>
       </c>
       <c r="J15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2077,19 +2021,19 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I16">
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2101,7 +2045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541E4620-502E-4E54-ACE2-123DD601DFC8}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -2125,25 +2069,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2160,19 +2104,19 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2189,19 +2133,19 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>259</v>
+      </c>
+      <c r="F3" t="s">
         <v>261</v>
       </c>
-      <c r="F3" t="s">
-        <v>263</v>
-      </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2218,19 +2162,19 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2247,19 +2191,19 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2276,19 +2220,19 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I6">
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -2305,19 +2249,19 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I7">
         <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2334,19 +2278,19 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I8">
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2363,19 +2307,19 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I9">
         <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2392,19 +2336,19 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I10">
         <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2421,19 +2365,19 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -2450,19 +2394,19 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F12" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I12">
         <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2479,19 +2423,19 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F13" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2508,19 +2452,19 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I14">
         <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2537,19 +2481,19 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F15" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I15">
         <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2566,19 +2510,19 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F16" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I16">
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2595,19 +2539,19 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F17" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2624,19 +2568,19 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F18" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2653,19 +2597,19 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F19" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I19">
         <v>10</v>
       </c>
       <c r="J19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2682,19 +2626,19 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I20">
         <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2711,19 +2655,19 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F21" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I21">
         <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2740,19 +2684,19 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F22" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I22">
         <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -2769,19 +2713,19 @@
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F23" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I23">
         <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -2798,19 +2742,19 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F24" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I24">
         <v>10</v>
       </c>
       <c r="J24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2827,19 +2771,19 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F25" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I25">
         <v>10</v>
       </c>
       <c r="J25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2856,19 +2800,19 @@
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I26">
         <v>10</v>
       </c>
       <c r="J26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2885,19 +2829,19 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F27" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I27">
         <v>10</v>
       </c>
       <c r="J27" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2914,19 +2858,19 @@
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F28" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I28">
         <v>10</v>
       </c>
       <c r="J28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -2943,19 +2887,19 @@
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H29" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I29">
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2990,25 +2934,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -3025,19 +2969,19 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3054,19 +2998,19 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3083,19 +3027,19 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4">
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3112,19 +3056,19 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3141,19 +3085,19 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3170,19 +3114,19 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3199,19 +3143,19 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3228,19 +3172,19 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3257,19 +3201,19 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F10" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3286,19 +3230,19 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -3334,25 +3278,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -3369,16 +3313,16 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3395,16 +3339,16 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3421,16 +3365,16 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4">
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3447,16 +3391,16 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I5">
         <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3473,16 +3417,16 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I6">
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3499,16 +3443,16 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I7">
         <v>0.1</v>
       </c>
       <c r="J7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3525,16 +3469,16 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I8">
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3551,16 +3495,16 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I9">
         <v>0.5</v>
       </c>
       <c r="J9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3577,16 +3521,16 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3603,16 +3547,16 @@
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3629,16 +3573,16 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3655,16 +3599,16 @@
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -3681,16 +3625,16 @@
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3707,19 +3651,19 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3736,16 +3680,16 @@
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I16">
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -3762,16 +3706,16 @@
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -3788,16 +3732,16 @@
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I18">
         <v>0.01</v>
       </c>
       <c r="J18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -3814,19 +3758,19 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I19">
         <v>0.01</v>
       </c>
       <c r="J19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3843,16 +3787,16 @@
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I20">
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -3869,16 +3813,16 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I21">
         <v>0.5</v>
       </c>
       <c r="J21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -3895,19 +3839,19 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I22">
         <v>0.01</v>
       </c>
       <c r="J22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -3924,16 +3868,16 @@
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I23">
         <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -3950,16 +3894,16 @@
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I24">
         <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3971,8 +3915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49756CD-7B89-4299-B487-83FA9AC75873}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3996,30 +3940,30 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
       </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -4028,22 +3972,22 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>298</v>
       </c>
       <c r="F2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I2">
         <v>0.01</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4060,16 +4004,16 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I3">
         <v>1E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4086,16 +4030,16 @@
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4">
         <v>1E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -4112,16 +4056,16 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I5">
         <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -4138,16 +4082,16 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I6">
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4164,19 +4108,19 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I7">
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4193,16 +4137,16 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I8">
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4219,16 +4163,16 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I9">
         <v>0.01</v>
       </c>
       <c r="J9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4245,16 +4189,16 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I10">
         <v>0.01</v>
       </c>
       <c r="J10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4271,16 +4215,16 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I11">
         <v>0.01</v>
       </c>
       <c r="J11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -4293,8 +4237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E27EF3F-1977-4DFD-AB2B-D5DA3F473BBD}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4317,25 +4261,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -4352,19 +4296,19 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4381,19 +4325,19 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4410,19 +4354,19 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -4439,19 +4383,19 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -4468,19 +4412,19 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4497,19 +4441,19 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4526,19 +4470,19 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4555,19 +4499,19 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4584,19 +4528,19 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4613,19 +4557,19 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -4642,19 +4586,19 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -4671,19 +4615,19 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -4700,19 +4644,19 @@
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -4729,19 +4673,19 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -4758,19 +4702,19 @@
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I16">
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -4787,19 +4731,19 @@
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -4816,19 +4760,19 @@
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -4845,19 +4789,19 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -4874,19 +4818,19 @@
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I20">
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -4903,19 +4847,19 @@
         <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F21" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I21">
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -4932,19 +4876,19 @@
         <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I22">
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -4961,19 +4905,19 @@
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -4990,19 +4934,19 @@
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I24">
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -5019,19 +4963,19 @@
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I25">
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -5048,19 +4992,19 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -5077,19 +5021,19 @@
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F27" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I27">
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -5106,19 +5050,19 @@
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I28">
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -5135,19 +5079,19 @@
         <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F29" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H29" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I29">
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -5164,19 +5108,19 @@
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F30" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I30">
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -5193,19 +5137,19 @@
         <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F31" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I31">
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -5222,19 +5166,19 @@
         <v>5</v>
       </c>
       <c r="E32" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F32" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I32">
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -5251,201 +5195,23 @@
         <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F33" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I33">
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21909002-3FEB-40D1-A6BE-6D67D597F061}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G1" t="s">
-        <v>155</v>
-      </c>
-      <c r="H1" t="s">
-        <v>156</v>
-      </c>
-      <c r="I1" t="s">
-        <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>300</v>
-      </c>
-      <c r="B2" s="1">
-        <v>378</v>
-      </c>
-      <c r="C2" s="1">
-        <v>378</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F2" t="s">
-        <v>301</v>
-      </c>
-      <c r="G2" t="s">
-        <v>302</v>
-      </c>
-      <c r="H2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>304</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>305</v>
-      </c>
-      <c r="F3" t="s">
-        <v>306</v>
-      </c>
-      <c r="G3" t="s">
-        <v>307</v>
-      </c>
-      <c r="H3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>309</v>
-      </c>
-      <c r="F4" t="s">
-        <v>310</v>
-      </c>
-      <c r="G4" t="s">
-        <v>311</v>
-      </c>
-      <c r="H4" t="s">
-        <v>153</v>
-      </c>
-      <c r="I4">
-        <v>1E-3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>204</v>
-      </c>
-      <c r="F5" t="s">
-        <v>313</v>
-      </c>
-      <c r="G5" t="s">
-        <v>314</v>
-      </c>
-      <c r="H5" t="s">
-        <v>153</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
no idea where the change happened
</commit_message>
<xml_diff>
--- a/data/Apple_AF_Steinfurt_wRisk_30.xlsx
+++ b/data/Apple_AF_Steinfurt_wRisk_30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\Project_report\Deliverables\D4.3_Model_Comparison\Apple_Agroforestry\Apple_Agroforestry\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193E747E-D065-4396-9BDD-DCBD4EBFDC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBF1340-833A-4EB6-9B0B-80081CAD6AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="298">
   <si>
     <t>variable</t>
   </si>
@@ -921,9 +921,6 @@
   </si>
   <si>
     <t>Data analyst;Agroforestry farming</t>
-  </si>
-  <si>
-    <t>tnorm_0_1</t>
   </si>
 </sst>
 </file>
@@ -3915,7 +3912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49756CD-7B89-4299-B487-83FA9AC75873}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -3972,7 +3969,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>298</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
         <v>162</v>
@@ -4237,8 +4234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E27EF3F-1977-4DFD-AB2B-D5DA3F473BBD}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
units and experts added
</commit_message>
<xml_diff>
--- a/data/Apple_AF_Steinfurt_wRisk_30.xlsx
+++ b/data/Apple_AF_Steinfurt_wRisk_30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\Project_report\Deliverables\D4.3_Model_Comparison\Apple_Agroforestry\Apple_Agroforestry\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBF1340-833A-4EB6-9B0B-80081CAD6AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C07B901-3D17-4000-93C1-507CDD81A782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="302">
   <si>
     <t>variable</t>
   </si>
@@ -485,9 +485,6 @@
     <t>numeric</t>
   </si>
   <si>
-    <t>Data analyst</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -518,9 +515,6 @@
     <t>Probability of extreme weather</t>
   </si>
   <si>
-    <t>Agroforestry farming</t>
-  </si>
-  <si>
     <t>chance_extreme_weather_t</t>
   </si>
   <si>
@@ -632,60 +626,12 @@
     <t>Risk that irrigation system needs repair</t>
   </si>
   <si>
-    <t>Percentage Repair cost of irrigation system compared to new</t>
-  </si>
-  <si>
     <t>€</t>
   </si>
   <si>
-    <t xml:space="preserve">Cost of pruning course for employee </t>
-  </si>
-  <si>
-    <t>Water use in frist three years of tree establishment</t>
-  </si>
-  <si>
-    <t>Water use in annual irrigation</t>
-  </si>
-  <si>
-    <t>Labour hours for pruning juvenile apple trees (year 1-5)</t>
-  </si>
-  <si>
-    <t>Labour hours for pruning juvenile apple trees (6-10)</t>
-  </si>
-  <si>
-    <t>Labour hours for pruning mature apple trees (year 11-15)</t>
-  </si>
-  <si>
-    <t>Labour hours for pruning mature apple trees (year 16 onwards)</t>
-  </si>
-  <si>
-    <t>Labour hours for root pruning trees</t>
-  </si>
-  <si>
-    <t>Labour hours for mowing the tree strips manually</t>
-  </si>
-  <si>
-    <t>Price of table apples</t>
-  </si>
-  <si>
-    <t>Price of intermediate quality apples</t>
-  </si>
-  <si>
     <t>€/kg</t>
   </si>
   <si>
-    <t xml:space="preserve">Price of juice apples </t>
-  </si>
-  <si>
-    <t>First apple yield, % of max. apple yield</t>
-  </si>
-  <si>
-    <t>Second stage apple yield, % of max. apple yield</t>
-  </si>
-  <si>
-    <t>Maximum apple yield</t>
-  </si>
-  <si>
     <t>Estimate 1 when apple trees produce first harvest</t>
   </si>
   <si>
@@ -698,114 +644,33 @@
     <t>Estimate 2 when apple trees reach second yield stage (for gompertz curve)</t>
   </si>
   <si>
-    <t>Labour cost for harvesting a kg of apples</t>
-  </si>
-  <si>
-    <t>Post Harvest loss of Apple</t>
-  </si>
-  <si>
-    <t>Percentage of total apple yield with table apple quality</t>
-  </si>
-  <si>
-    <t>Percentage of intermediate quality apples</t>
-  </si>
-  <si>
-    <t>Time spent discussing goals with consultants, planning AF system and other planning work done by farmer</t>
-  </si>
-  <si>
     <t>h</t>
   </si>
   <si>
-    <t>Total payment of hired agroforestry consultant</t>
-  </si>
-  <si>
-    <t>Cost of labour</t>
-  </si>
-  <si>
     <t>€/h</t>
   </si>
   <si>
-    <t>Time spent on LEADER application for financial support</t>
-  </si>
-  <si>
-    <t>Time spent on ES3 application for financial support</t>
-  </si>
-  <si>
-    <t>Additional expected labour for managing arable crops in AF system</t>
-  </si>
-  <si>
-    <t>Cost of irrigation water</t>
-  </si>
-  <si>
     <t>€/l</t>
   </si>
   <si>
-    <t>Labour hours for preparing planting holes</t>
-  </si>
-  <si>
     <t>h/tree</t>
   </si>
   <si>
-    <t>Labour hours of planting tree</t>
-  </si>
-  <si>
-    <t>Price per apple tree (tree only)</t>
-  </si>
-  <si>
-    <t>Cost of mesh for protection against vole damage</t>
-  </si>
-  <si>
-    <t>Cost of mesh for protection against deer browsing</t>
-  </si>
-  <si>
-    <t>Cost of adding fleece to tree base for weed suppression</t>
-  </si>
-  <si>
-    <t>Cost of buying and installing irrigation system</t>
-  </si>
-  <si>
-    <t>Water use right after planting tree</t>
-  </si>
-  <si>
     <t>l/tree</t>
   </si>
   <si>
-    <t>Compost used at time of planting</t>
-  </si>
-  <si>
-    <t>Price of compost</t>
-  </si>
-  <si>
-    <t>Cost of installing pheromone dispensers</t>
-  </si>
-  <si>
-    <t>Total area of tree rows (wooded area) in AF system</t>
-  </si>
-  <si>
     <t>Number of apple trees planted in AF system</t>
   </si>
   <si>
     <t>ha</t>
   </si>
   <si>
-    <t>Labour hours for measuring field with GPS, identifying placement of trees</t>
-  </si>
-  <si>
     <t>Estimate 1 when reduced produce first harvest of crop</t>
   </si>
   <si>
     <t>Estimate 2 when reduced produce second harvest of crop</t>
   </si>
   <si>
-    <t>Percentage max first reduction</t>
-  </si>
-  <si>
-    <t>Percentage max second reduction</t>
-  </si>
-  <si>
-    <t>Agroforestry farming;Data analyst</t>
-  </si>
-  <si>
     <t>t/ha</t>
   </si>
   <si>
@@ -920,7 +785,154 @@
     <t>Crop Coefficients</t>
   </si>
   <si>
-    <t>Data analyst;Agroforestry farming</t>
+    <t>Total area of tree rows (wooded area) in AF system [ha]</t>
+  </si>
+  <si>
+    <t>Labour hours for measuring field with GPS, identifying placement of trees [h]</t>
+  </si>
+  <si>
+    <t>Cost of irrigation water [€/l]</t>
+  </si>
+  <si>
+    <t>Labour hours for preparing planting holes [h/tree]</t>
+  </si>
+  <si>
+    <t>Labour hours of planting tree [h/tree]</t>
+  </si>
+  <si>
+    <t>Price per apple tree (tree only) [h/tree]</t>
+  </si>
+  <si>
+    <t>Cost of mesh for protection against vole damage [h/tree]</t>
+  </si>
+  <si>
+    <t>Cost of mesh for protection against deer browsing [h/tree]</t>
+  </si>
+  <si>
+    <t>Cost of adding fleece to tree base for weed suppression [h/tree]</t>
+  </si>
+  <si>
+    <t>Water use right after planting tree [l/tree]</t>
+  </si>
+  <si>
+    <t>Cost of installing pheromone dispensers [l/tree]</t>
+  </si>
+  <si>
+    <t>Compost used at time of planting [l/tree]</t>
+  </si>
+  <si>
+    <t>Price of compost [€/l]</t>
+  </si>
+  <si>
+    <t>Cost of buying and installing irrigation system [€]</t>
+  </si>
+  <si>
+    <t>Additional expected labour for managing arable crops in AF system [%]</t>
+  </si>
+  <si>
+    <t>Cost of labour [€/h]</t>
+  </si>
+  <si>
+    <t>Total payment of hired agroforestry consultant [€]</t>
+  </si>
+  <si>
+    <t>Time spent on ES3 application for financial support [h]</t>
+  </si>
+  <si>
+    <t>Time spent on LEADER application for financial support [h]</t>
+  </si>
+  <si>
+    <t>Time spent discussing goals with consultants, planning AF system and other planning work done by farmer [h]</t>
+  </si>
+  <si>
+    <t>Cost of pruning course for employee [€]</t>
+  </si>
+  <si>
+    <t>Water use in annual irrigation  [l/tree]</t>
+  </si>
+  <si>
+    <t>Water use in first three years of tree establishment  [l/tree]</t>
+  </si>
+  <si>
+    <t>Labour hours for pruning juvenile apple trees (year 1-5) [h]</t>
+  </si>
+  <si>
+    <t>Labour hours for pruning juvenile apple trees (6-10) [h]</t>
+  </si>
+  <si>
+    <t>Labour hours for pruning mature apple trees (year 11-15) [h]</t>
+  </si>
+  <si>
+    <t>Labour hours for pruning mature apple trees (year 16 onwards) [h]</t>
+  </si>
+  <si>
+    <t>Labour hours for root pruning trees [h]</t>
+  </si>
+  <si>
+    <t>Labour hours for mowing the tree strips manually [h]</t>
+  </si>
+  <si>
+    <t>First apple yield, % of max. apple yield [%]</t>
+  </si>
+  <si>
+    <t>Maximum apple yield [kg/tree]</t>
+  </si>
+  <si>
+    <t>Second stage apple yield, % of max. apple yield [%]</t>
+  </si>
+  <si>
+    <t>Labour cost for harvesting a kg of apples [€/kg]</t>
+  </si>
+  <si>
+    <t>Post Harvest loss of Apple [%]</t>
+  </si>
+  <si>
+    <t>Price of table apples [€/kg]</t>
+  </si>
+  <si>
+    <t>Price of intermediate quality apples [€/kg]</t>
+  </si>
+  <si>
+    <t>Price of juice apples [€/kg]</t>
+  </si>
+  <si>
+    <t>Percentage of total apple yield with table apple quality [%]</t>
+  </si>
+  <si>
+    <t>Percentage of intermediate quality apples [%]</t>
+  </si>
+  <si>
+    <t>Percentage Repair cost of irrigation system compared to new [%]</t>
+  </si>
+  <si>
+    <t>Percentage max first reduction [%]</t>
+  </si>
+  <si>
+    <t>Percentage max second reduction [%]</t>
+  </si>
+  <si>
+    <t>Data analyst;Market analyst</t>
+  </si>
+  <si>
+    <t>Decision-maker;Agroforestry farmer;Policy-maker;Data analyst;Market analyst</t>
+  </si>
+  <si>
+    <t>Agroforestry farmer;Data analyst</t>
+  </si>
+  <si>
+    <t>Data analyst;Agroforestry farmer;Market analyst;Policy-maker</t>
+  </si>
+  <si>
+    <t>Data analyst;Agroforestry farmer</t>
+  </si>
+  <si>
+    <t>Agroforestry farmer;Data analyst;Policy-maker</t>
+  </si>
+  <si>
+    <t>Agroforestry farmer;Data analyst;Market analyst;Policy-maker</t>
+  </si>
+  <si>
+    <t>Data analyst;Market analyst;Policy-maker;Agroforestry farmer</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1344,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>295</v>
+        <v>250</v>
       </c>
       <c r="B7" t="s">
         <v>140</v>
@@ -1340,7 +1352,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>296</v>
+        <v>251</v>
       </c>
       <c r="B8" t="s">
         <v>139</v>
@@ -1355,14 +1367,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92018703-4177-49D8-B09E-62560F009CDF}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1385,19 +1398,19 @@
         <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" t="s">
         <v>153</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>156</v>
-      </c>
-      <c r="K1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1426,7 +1439,7 @@
         <v>1000</v>
       </c>
       <c r="J2" t="s">
-        <v>163</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1446,13 +1459,13 @@
         <v>145</v>
       </c>
       <c r="F3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" t="s">
         <v>158</v>
       </c>
-      <c r="G3" t="s">
-        <v>159</v>
-      </c>
       <c r="H3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1481,13 +1494,13 @@
         <v>146</v>
       </c>
       <c r="H4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>152</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1504,10 +1517,10 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>252</v>
+        <v>211</v>
       </c>
       <c r="F5" t="s">
-        <v>294</v>
+        <v>249</v>
       </c>
       <c r="H5" t="s">
         <v>151</v>
@@ -1516,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>152</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1548,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>152</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -1561,12 +1574,13 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1589,19 +1603,19 @@
         <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" t="s">
         <v>153</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>156</v>
-      </c>
-      <c r="K1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1618,10 +1632,10 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" t="s">
         <v>252</v>
-      </c>
-      <c r="F2" t="s">
-        <v>250</v>
       </c>
       <c r="H2" t="s">
         <v>151</v>
@@ -1630,7 +1644,7 @@
         <v>0.1</v>
       </c>
       <c r="J2" t="s">
-        <v>163</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1647,7 +1661,7 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>251</v>
+        <v>210</v>
       </c>
       <c r="H3" t="s">
         <v>151</v>
@@ -1656,7 +1670,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>163</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1676,13 +1690,13 @@
         <v>253</v>
       </c>
       <c r="H4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1699,19 +1713,19 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="F5" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="H5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I5">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J5" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1728,19 +1742,19 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="F6" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="H6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I6">
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1757,19 +1771,19 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="F7" t="s">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="H7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I7">
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1786,19 +1800,19 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="F8" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="H8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1815,19 +1829,19 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="F9" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="H9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1844,19 +1858,19 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="F10" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="H10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1873,19 +1887,19 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="F11" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="H11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I11">
         <v>0.1</v>
       </c>
       <c r="J11" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1902,19 +1916,19 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F12" t="s">
-        <v>244</v>
+        <v>265</v>
       </c>
       <c r="H12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I12">
         <v>100</v>
       </c>
       <c r="J12" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1931,19 +1945,19 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
       <c r="F13" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="H13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1960,19 +1974,19 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
       <c r="F14" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="H14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1989,10 +2003,10 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="F15" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="H15" t="s">
         <v>151</v>
@@ -2001,7 +2015,7 @@
         <v>0.1</v>
       </c>
       <c r="J15" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2018,19 +2032,19 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
       <c r="F16" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="H16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I16">
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -2042,8 +2056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541E4620-502E-4E54-ACE2-123DD601DFC8}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2072,19 +2086,19 @@
         <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" t="s">
         <v>153</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>156</v>
-      </c>
-      <c r="K1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2101,19 +2115,19 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F2" t="s">
-        <v>260</v>
+        <v>215</v>
       </c>
       <c r="H2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>163</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2130,19 +2144,19 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F3" t="s">
-        <v>261</v>
+        <v>216</v>
       </c>
       <c r="H3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>163</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2159,19 +2173,19 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F4" t="s">
-        <v>262</v>
+        <v>217</v>
       </c>
       <c r="H4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>163</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2188,19 +2202,19 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="F5" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="H5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>163</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2217,19 +2231,19 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F6" t="s">
-        <v>267</v>
+        <v>222</v>
       </c>
       <c r="H6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I6">
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>163</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -2246,19 +2260,19 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>266</v>
+        <v>221</v>
       </c>
       <c r="F7" t="s">
-        <v>269</v>
+        <v>224</v>
       </c>
       <c r="H7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I7">
         <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2275,19 +2289,19 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F8" t="s">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="H8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I8">
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2304,19 +2318,19 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F9" t="s">
-        <v>271</v>
+        <v>226</v>
       </c>
       <c r="H9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I9">
         <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2333,19 +2347,19 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F10" t="s">
-        <v>272</v>
+        <v>227</v>
       </c>
       <c r="H10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I10">
         <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2362,19 +2376,19 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F11" t="s">
-        <v>274</v>
+        <v>229</v>
       </c>
       <c r="H11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -2391,19 +2405,19 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F12" t="s">
-        <v>267</v>
+        <v>222</v>
       </c>
       <c r="H12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I12">
         <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2420,19 +2434,19 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>266</v>
+        <v>221</v>
       </c>
       <c r="F13" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="H13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2449,19 +2463,19 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F14" t="s">
-        <v>290</v>
+        <v>245</v>
       </c>
       <c r="H14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I14">
         <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2478,19 +2492,19 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F15" t="s">
-        <v>291</v>
+        <v>246</v>
       </c>
       <c r="H15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I15">
         <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2507,19 +2521,19 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F16" t="s">
-        <v>292</v>
+        <v>247</v>
       </c>
       <c r="H16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I16">
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2536,19 +2550,19 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F17" t="s">
-        <v>275</v>
+        <v>230</v>
       </c>
       <c r="H17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2565,19 +2579,19 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F18" t="s">
-        <v>268</v>
+        <v>223</v>
       </c>
       <c r="H18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2594,19 +2608,19 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>266</v>
+        <v>221</v>
       </c>
       <c r="F19" t="s">
-        <v>284</v>
+        <v>239</v>
       </c>
       <c r="H19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I19">
         <v>10</v>
       </c>
       <c r="J19" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2623,19 +2637,19 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F20" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="H20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I20">
         <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2652,19 +2666,19 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F21" t="s">
-        <v>286</v>
+        <v>241</v>
       </c>
       <c r="H21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I21">
         <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2681,19 +2695,19 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F22" t="s">
-        <v>287</v>
+        <v>242</v>
       </c>
       <c r="H22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I22">
         <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -2710,19 +2724,19 @@
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F23" t="s">
-        <v>276</v>
+        <v>231</v>
       </c>
       <c r="H23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I23">
         <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -2739,19 +2753,19 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F24" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="H24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I24">
         <v>10</v>
       </c>
       <c r="J24" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2768,19 +2782,19 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>266</v>
+        <v>221</v>
       </c>
       <c r="F25" t="s">
-        <v>278</v>
+        <v>233</v>
       </c>
       <c r="H25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I25">
         <v>10</v>
       </c>
       <c r="J25" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2797,19 +2811,19 @@
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F26" t="s">
-        <v>279</v>
+        <v>234</v>
       </c>
       <c r="H26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I26">
         <v>10</v>
       </c>
       <c r="J26" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2826,19 +2840,19 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F27" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="H27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I27">
         <v>10</v>
       </c>
       <c r="J27" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2855,19 +2869,19 @@
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F28" t="s">
-        <v>281</v>
+        <v>236</v>
       </c>
       <c r="H28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I28">
         <v>10</v>
       </c>
       <c r="J28" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -2884,19 +2898,19 @@
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="F29" t="s">
-        <v>283</v>
+        <v>238</v>
       </c>
       <c r="H29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I29">
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2908,13 +2922,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D887141-305C-4556-91D4-D86C0CE94422}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="88.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -2937,19 +2952,19 @@
         <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" t="s">
         <v>153</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>156</v>
-      </c>
-      <c r="K1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2966,19 +2981,19 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="F2" t="s">
-        <v>227</v>
+        <v>271</v>
       </c>
       <c r="H2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2995,19 +3010,19 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F3" t="s">
-        <v>229</v>
+        <v>268</v>
       </c>
       <c r="H3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3024,19 +3039,19 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="F4" t="s">
-        <v>230</v>
+        <v>267</v>
       </c>
       <c r="H4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I4">
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3053,19 +3068,19 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="F5" t="s">
-        <v>233</v>
+        <v>269</v>
       </c>
       <c r="H5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3082,19 +3097,19 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="F6" t="s">
-        <v>232</v>
+        <v>270</v>
       </c>
       <c r="H6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3114,16 +3129,16 @@
         <v>145</v>
       </c>
       <c r="F7" t="s">
-        <v>234</v>
+        <v>266</v>
       </c>
       <c r="H7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3140,19 +3155,19 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
       <c r="F8" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="H8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3169,19 +3184,19 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
       <c r="F9" t="s">
-        <v>293</v>
+        <v>248</v>
       </c>
       <c r="H9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3198,19 +3213,19 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
       <c r="F10" t="s">
-        <v>288</v>
+        <v>243</v>
       </c>
       <c r="H10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3227,19 +3242,19 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
       <c r="F11" t="s">
-        <v>273</v>
+        <v>228</v>
       </c>
       <c r="H11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -3252,13 +3267,14 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="J17" sqref="J17:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="62.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -3281,19 +3297,19 @@
         <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" t="s">
         <v>153</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>156</v>
-      </c>
-      <c r="K1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -3310,16 +3326,16 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>203</v>
+        <v>272</v>
       </c>
       <c r="H2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3336,16 +3352,16 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>204</v>
+        <v>274</v>
       </c>
       <c r="H3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3362,16 +3378,16 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>205</v>
+        <v>273</v>
       </c>
       <c r="H4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I4">
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3388,16 +3404,16 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>206</v>
+        <v>275</v>
       </c>
       <c r="H5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I5">
         <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3414,16 +3430,16 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>207</v>
+        <v>276</v>
       </c>
       <c r="H6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I6">
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3440,16 +3456,16 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>208</v>
+        <v>277</v>
       </c>
       <c r="H7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I7">
         <v>0.1</v>
       </c>
       <c r="J7" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3466,16 +3482,16 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>209</v>
+        <v>278</v>
       </c>
       <c r="H8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I8">
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3492,16 +3508,16 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>210</v>
+        <v>279</v>
       </c>
       <c r="H9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I9">
         <v>0.5</v>
       </c>
       <c r="J9" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3518,16 +3534,16 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>211</v>
+        <v>280</v>
       </c>
       <c r="H10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3544,7 +3560,7 @@
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="H11" t="s">
         <v>151</v>
@@ -3553,7 +3569,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3570,7 +3586,7 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="H12" t="s">
         <v>151</v>
@@ -3579,7 +3595,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3596,7 +3612,7 @@
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="H13" t="s">
         <v>151</v>
@@ -3605,7 +3621,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -3622,7 +3638,7 @@
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="H14" t="s">
         <v>151</v>
@@ -3631,7 +3647,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3651,16 +3667,16 @@
         <v>145</v>
       </c>
       <c r="F15" t="s">
-        <v>216</v>
+        <v>281</v>
       </c>
       <c r="H15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3677,16 +3693,16 @@
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>217</v>
+        <v>283</v>
       </c>
       <c r="H16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I16">
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -3703,16 +3719,16 @@
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>218</v>
+        <v>282</v>
       </c>
       <c r="H17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -3729,16 +3745,16 @@
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>223</v>
+        <v>284</v>
       </c>
       <c r="H18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I18">
         <v>0.01</v>
       </c>
       <c r="J18" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -3758,16 +3774,16 @@
         <v>145</v>
       </c>
       <c r="F19" t="s">
-        <v>224</v>
+        <v>285</v>
       </c>
       <c r="H19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I19">
         <v>0.01</v>
       </c>
       <c r="J19" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3784,16 +3800,16 @@
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>212</v>
+        <v>286</v>
       </c>
       <c r="H20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I20">
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -3810,16 +3826,16 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>213</v>
+        <v>287</v>
       </c>
       <c r="H21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I21">
         <v>0.5</v>
       </c>
       <c r="J21" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -3836,19 +3852,19 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="F22" t="s">
-        <v>215</v>
+        <v>288</v>
       </c>
       <c r="H22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I22">
         <v>0.01</v>
       </c>
       <c r="J22" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -3865,16 +3881,16 @@
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>225</v>
+        <v>289</v>
       </c>
       <c r="H23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I23">
         <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -3891,16 +3907,16 @@
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>226</v>
+        <v>290</v>
       </c>
       <c r="H24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I24">
         <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -3912,14 +3928,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49756CD-7B89-4299-B487-83FA9AC75873}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3943,24 +3959,24 @@
         <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" t="s">
         <v>153</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>156</v>
-      </c>
-      <c r="K1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3972,19 +3988,19 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I2">
         <v>0.01</v>
       </c>
       <c r="J2" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4001,16 +4017,16 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I3">
         <v>1E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4027,16 +4043,16 @@
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I4">
         <v>1E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -4053,16 +4069,16 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I5">
         <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -4079,16 +4095,16 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I6">
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4108,16 +4124,16 @@
         <v>145</v>
       </c>
       <c r="F7" t="s">
-        <v>201</v>
+        <v>291</v>
       </c>
       <c r="H7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I7">
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>163</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4134,7 +4150,7 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>254</v>
+        <v>212</v>
       </c>
       <c r="H8" t="s">
         <v>151</v>
@@ -4143,7 +4159,7 @@
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>152</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4160,7 +4176,7 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>255</v>
+        <v>213</v>
       </c>
       <c r="H9" t="s">
         <v>151</v>
@@ -4169,7 +4185,7 @@
         <v>0.01</v>
       </c>
       <c r="J9" t="s">
-        <v>152</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4186,16 +4202,16 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>256</v>
+        <v>292</v>
       </c>
       <c r="H10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I10">
         <v>0.01</v>
       </c>
       <c r="J10" t="s">
-        <v>152</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4212,16 +4228,16 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>257</v>
+        <v>293</v>
       </c>
       <c r="H11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I11">
         <v>0.01</v>
       </c>
       <c r="J11" t="s">
-        <v>152</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -4234,8 +4250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E27EF3F-1977-4DFD-AB2B-D5DA3F473BBD}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4264,19 +4280,19 @@
         <v>142</v>
       </c>
       <c r="G1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" t="s">
         <v>153</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>156</v>
-      </c>
-      <c r="K1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -4296,7 +4312,7 @@
         <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H2" t="s">
         <v>151</v>
@@ -4305,7 +4321,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4325,7 +4341,7 @@
         <v>145</v>
       </c>
       <c r="F3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H3" t="s">
         <v>151</v>
@@ -4334,7 +4350,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4354,7 +4370,7 @@
         <v>145</v>
       </c>
       <c r="F4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H4" t="s">
         <v>151</v>
@@ -4363,7 +4379,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -4383,7 +4399,7 @@
         <v>145</v>
       </c>
       <c r="F5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H5" t="s">
         <v>151</v>
@@ -4392,7 +4408,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -4412,7 +4428,7 @@
         <v>145</v>
       </c>
       <c r="F6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H6" t="s">
         <v>151</v>
@@ -4421,7 +4437,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4441,7 +4457,7 @@
         <v>145</v>
       </c>
       <c r="F7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H7" t="s">
         <v>151</v>
@@ -4450,7 +4466,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4470,7 +4486,7 @@
         <v>145</v>
       </c>
       <c r="F8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H8" t="s">
         <v>151</v>
@@ -4479,7 +4495,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4499,7 +4515,7 @@
         <v>145</v>
       </c>
       <c r="F9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H9" t="s">
         <v>151</v>
@@ -4508,7 +4524,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4528,7 +4544,7 @@
         <v>145</v>
       </c>
       <c r="F10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H10" t="s">
         <v>151</v>
@@ -4537,7 +4553,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4557,7 +4573,7 @@
         <v>145</v>
       </c>
       <c r="F11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H11" t="s">
         <v>151</v>
@@ -4566,7 +4582,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -4586,7 +4602,7 @@
         <v>145</v>
       </c>
       <c r="F12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H12" t="s">
         <v>151</v>
@@ -4595,7 +4611,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -4615,7 +4631,7 @@
         <v>145</v>
       </c>
       <c r="F13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H13" t="s">
         <v>151</v>
@@ -4624,7 +4640,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -4644,7 +4660,7 @@
         <v>145</v>
       </c>
       <c r="F14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H14" t="s">
         <v>151</v>
@@ -4653,7 +4669,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -4673,7 +4689,7 @@
         <v>145</v>
       </c>
       <c r="F15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H15" t="s">
         <v>151</v>
@@ -4682,7 +4698,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -4702,7 +4718,7 @@
         <v>145</v>
       </c>
       <c r="F16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H16" t="s">
         <v>151</v>
@@ -4711,7 +4727,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -4731,7 +4747,7 @@
         <v>145</v>
       </c>
       <c r="F17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H17" t="s">
         <v>151</v>
@@ -4740,7 +4756,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -4760,7 +4776,7 @@
         <v>145</v>
       </c>
       <c r="F18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H18" t="s">
         <v>151</v>
@@ -4769,7 +4785,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -4789,7 +4805,7 @@
         <v>145</v>
       </c>
       <c r="F19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H19" t="s">
         <v>151</v>
@@ -4798,7 +4814,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -4818,7 +4834,7 @@
         <v>145</v>
       </c>
       <c r="F20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H20" t="s">
         <v>151</v>
@@ -4827,7 +4843,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -4847,7 +4863,7 @@
         <v>145</v>
       </c>
       <c r="F21" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H21" t="s">
         <v>151</v>
@@ -4856,7 +4872,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -4876,7 +4892,7 @@
         <v>145</v>
       </c>
       <c r="F22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H22" t="s">
         <v>151</v>
@@ -4885,7 +4901,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -4905,7 +4921,7 @@
         <v>145</v>
       </c>
       <c r="F23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H23" t="s">
         <v>151</v>
@@ -4914,7 +4930,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -4934,7 +4950,7 @@
         <v>145</v>
       </c>
       <c r="F24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H24" t="s">
         <v>151</v>
@@ -4943,7 +4959,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -4963,7 +4979,7 @@
         <v>145</v>
       </c>
       <c r="F25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H25" t="s">
         <v>151</v>
@@ -4972,7 +4988,7 @@
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -4992,7 +5008,7 @@
         <v>145</v>
       </c>
       <c r="F26" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H26" t="s">
         <v>151</v>
@@ -5001,7 +5017,7 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -5021,7 +5037,7 @@
         <v>145</v>
       </c>
       <c r="F27" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H27" t="s">
         <v>151</v>
@@ -5030,7 +5046,7 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -5050,7 +5066,7 @@
         <v>145</v>
       </c>
       <c r="F28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H28" t="s">
         <v>151</v>
@@ -5059,7 +5075,7 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -5079,7 +5095,7 @@
         <v>145</v>
       </c>
       <c r="F29" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H29" t="s">
         <v>151</v>
@@ -5088,7 +5104,7 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -5108,7 +5124,7 @@
         <v>145</v>
       </c>
       <c r="F30" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H30" t="s">
         <v>151</v>
@@ -5117,7 +5133,7 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -5137,7 +5153,7 @@
         <v>145</v>
       </c>
       <c r="F31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H31" t="s">
         <v>151</v>
@@ -5146,7 +5162,7 @@
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -5166,7 +5182,7 @@
         <v>145</v>
       </c>
       <c r="F32" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H32" t="s">
         <v>151</v>
@@ -5175,7 +5191,7 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -5195,7 +5211,7 @@
         <v>145</v>
       </c>
       <c r="F33" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H33" t="s">
         <v>151</v>
@@ -5204,7 +5220,7 @@
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor edits to expertise list
</commit_message>
<xml_diff>
--- a/data/Apple_AF_Steinfurt_wRisk_30.xlsx
+++ b/data/Apple_AF_Steinfurt_wRisk_30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\Project_report\Deliverables\D4.3_Model_Comparison\Apple_Agroforestry\Apple_Agroforestry\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C07B901-3D17-4000-93C1-507CDD81A782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEE6C6C-311D-4403-B2F3-A93263C221A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="2" r:id="rId1"/>
@@ -911,28 +911,28 @@
     <t>Percentage max second reduction [%]</t>
   </si>
   <si>
-    <t>Data analyst;Market analyst</t>
-  </si>
-  <si>
     <t>Decision-maker;Agroforestry farmer;Policy-maker;Data analyst;Market analyst</t>
   </si>
   <si>
-    <t>Agroforestry farmer;Data analyst</t>
-  </si>
-  <si>
-    <t>Data analyst;Agroforestry farmer;Market analyst;Policy-maker</t>
-  </si>
-  <si>
-    <t>Data analyst;Agroforestry farmer</t>
-  </si>
-  <si>
-    <t>Agroforestry farmer;Data analyst;Policy-maker</t>
-  </si>
-  <si>
-    <t>Agroforestry farmer;Data analyst;Market analyst;Policy-maker</t>
-  </si>
-  <si>
-    <t>Data analyst;Market analyst;Policy-maker;Agroforestry farmer</t>
+    <t>Data analyst;Agroforestry farmer;Market analyst;Policy-maker;Decision-maker</t>
+  </si>
+  <si>
+    <t>Data analyst;Market analyst;Policy-maker;Agroforestry farmer;Decision-maker</t>
+  </si>
+  <si>
+    <t>Data analyst;Agroforestry farmer;Decision-maker</t>
+  </si>
+  <si>
+    <t>Agroforestry farmer;Data analyst;Policy-maker;Decision-maker</t>
+  </si>
+  <si>
+    <t>Agroforestry farmer;Data analyst;Decision-maker</t>
+  </si>
+  <si>
+    <t>Agroforestry farmer;Data analyst;Market analyst;Policy-maker;Decision-maker</t>
+  </si>
+  <si>
+    <t>Data analyst;Market analyst;Decision-maker</t>
   </si>
 </sst>
 </file>
@@ -1367,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92018703-4177-49D8-B09E-62560F009CDF}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1439,7 +1439,7 @@
         <v>1000</v>
       </c>
       <c r="J2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1471,7 +1471,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1500,7 +1500,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1529,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1561,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -1574,7 +1574,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J4" sqref="J4:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1644,7 +1644,7 @@
         <v>0.1</v>
       </c>
       <c r="J2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1670,7 +1670,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1696,7 +1696,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1725,7 +1725,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J5" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1754,7 +1754,7 @@
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1783,7 +1783,7 @@
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1812,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1841,7 +1841,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1870,7 +1870,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1899,7 +1899,7 @@
         <v>0.1</v>
       </c>
       <c r="J11" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1928,7 +1928,7 @@
         <v>100</v>
       </c>
       <c r="J12" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1957,7 +1957,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1986,7 +1986,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2015,7 +2015,7 @@
         <v>0.1</v>
       </c>
       <c r="J15" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2044,7 +2044,7 @@
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -2056,8 +2056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541E4620-502E-4E54-ACE2-123DD601DFC8}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2156,7 +2156,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2185,7 +2185,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2214,7 +2214,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2243,7 +2243,7 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -2301,7 +2301,7 @@
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2330,7 +2330,7 @@
         <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2359,7 +2359,7 @@
         <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2417,7 +2417,7 @@
         <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2475,7 +2475,7 @@
         <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2504,7 +2504,7 @@
         <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2533,7 +2533,7 @@
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2591,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2649,7 +2649,7 @@
         <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2678,7 +2678,7 @@
         <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2707,7 +2707,7 @@
         <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -2765,7 +2765,7 @@
         <v>10</v>
       </c>
       <c r="J24" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2823,7 +2823,7 @@
         <v>10</v>
       </c>
       <c r="J26" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2852,7 +2852,7 @@
         <v>10</v>
       </c>
       <c r="J27" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2881,7 +2881,7 @@
         <v>10</v>
       </c>
       <c r="J28" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -2993,7 +2993,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3022,7 +3022,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3051,7 +3051,7 @@
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3080,7 +3080,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3109,7 +3109,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3138,7 +3138,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3167,7 +3167,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3196,7 +3196,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3225,7 +3225,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3254,7 +3254,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -3335,7 +3335,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3361,7 +3361,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3387,7 +3387,7 @@
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3413,7 +3413,7 @@
         <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3439,7 +3439,7 @@
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3465,7 +3465,7 @@
         <v>0.1</v>
       </c>
       <c r="J7" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3491,7 +3491,7 @@
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3517,7 +3517,7 @@
         <v>0.5</v>
       </c>
       <c r="J9" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3543,7 +3543,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3569,7 +3569,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3595,7 +3595,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3621,7 +3621,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -3647,7 +3647,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3676,7 +3676,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3702,7 +3702,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -4159,7 +4159,7 @@
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4185,7 +4185,7 @@
         <v>0.01</v>
       </c>
       <c r="J9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4211,7 +4211,7 @@
         <v>0.01</v>
       </c>
       <c r="J10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4237,7 +4237,7 @@
         <v>0.01</v>
       </c>
       <c r="J11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -4250,8 +4250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E27EF3F-1977-4DFD-AB2B-D5DA3F473BBD}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4321,7 +4321,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4350,7 +4350,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4379,7 +4379,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -4408,7 +4408,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -4437,7 +4437,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4466,7 +4466,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4495,7 +4495,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4524,7 +4524,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4553,7 +4553,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4582,7 +4582,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -4611,7 +4611,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -4640,7 +4640,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -4669,7 +4669,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -4698,7 +4698,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -4727,7 +4727,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -4756,7 +4756,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -4785,7 +4785,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -4814,7 +4814,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -4843,7 +4843,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -4872,7 +4872,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -4901,7 +4901,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -4930,7 +4930,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -4959,7 +4959,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -4988,7 +4988,7 @@
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -5017,7 +5017,7 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -5046,7 +5046,7 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -5075,7 +5075,7 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -5104,7 +5104,7 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -5133,7 +5133,7 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -5162,7 +5162,7 @@
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -5191,7 +5191,7 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -5220,7 +5220,7 @@
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor update to expertise category
</commit_message>
<xml_diff>
--- a/data/Apple_AF_Steinfurt_wRisk_30.xlsx
+++ b/data/Apple_AF_Steinfurt_wRisk_30.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Downloads\Apple_Agroforestry\Apple_Agroforestry\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\UK_visa_docs\Apple\Apple_Agroforestry\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B54E87-7E68-4624-80AB-88D05B89D5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6390DAD1-1A4A-4AC1-830F-E3A7EB9E46C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="2" r:id="rId1"/>
@@ -908,9 +908,6 @@
     <t>Percentage max second reduction [%]</t>
   </si>
   <si>
-    <t>Decision-maker;Agroforestry farmer;Policy-maker;Data analyst;Market analyst</t>
-  </si>
-  <si>
     <t>Price per apple tree (tree only) [€/tree]</t>
   </si>
   <si>
@@ -969,6 +966,9 @@
   </si>
   <si>
     <t>Agroforestry farmer;Data analyst;Market analyst;Policy-maker</t>
+  </si>
+  <si>
+    <t>Agroforestry farmer;Policy-maker;Data analyst;Market analyst</t>
   </si>
 </sst>
 </file>
@@ -1410,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92018703-4177-49D8-B09E-62560F009CDF}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1482,7 +1482,7 @@
         <v>1000</v>
       </c>
       <c r="J2" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1514,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1543,7 +1543,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1572,7 +1572,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1604,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -1687,12 +1687,12 @@
         <v>0.1</v>
       </c>
       <c r="J2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B3">
         <v>0.5</v>
@@ -1704,10 +1704,10 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H3" t="s">
         <v>151</v>
@@ -1716,7 +1716,7 @@
         <v>0.1</v>
       </c>
       <c r="J3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1742,7 +1742,7 @@
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1797,7 +1797,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1826,7 +1826,7 @@
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1855,7 +1855,7 @@
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1875,7 +1875,7 @@
         <v>208</v>
       </c>
       <c r="F9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H9" t="s">
         <v>159</v>
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1913,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1942,7 +1942,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1971,7 +1971,7 @@
         <v>0.1</v>
       </c>
       <c r="J12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2000,7 +2000,7 @@
         <v>100</v>
       </c>
       <c r="J13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2029,12 +2029,12 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B15">
         <v>3500</v>
@@ -2049,7 +2049,7 @@
         <v>199</v>
       </c>
       <c r="F15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H15" t="s">
         <v>159</v>
@@ -2058,7 +2058,7 @@
         <v>100</v>
       </c>
       <c r="J15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2087,7 +2087,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2116,7 +2116,7 @@
         <v>0.1</v>
       </c>
       <c r="J17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2145,7 +2145,7 @@
         <v>10</v>
       </c>
       <c r="J18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -2228,7 +2228,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2257,7 +2257,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2286,7 +2286,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2315,7 +2315,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2344,7 +2344,7 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -2373,7 +2373,7 @@
         <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2431,7 +2431,7 @@
         <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2460,7 +2460,7 @@
         <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2489,7 +2489,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -2518,7 +2518,7 @@
         <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2547,7 +2547,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2576,7 +2576,7 @@
         <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2605,7 +2605,7 @@
         <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2634,7 +2634,7 @@
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2663,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2692,7 +2692,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2721,7 +2721,7 @@
         <v>10</v>
       </c>
       <c r="J19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2750,7 +2750,7 @@
         <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2779,7 +2779,7 @@
         <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2808,7 +2808,7 @@
         <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -2837,7 +2837,7 @@
         <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -2866,7 +2866,7 @@
         <v>10</v>
       </c>
       <c r="J24" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2895,7 +2895,7 @@
         <v>10</v>
       </c>
       <c r="J25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2924,7 +2924,7 @@
         <v>10</v>
       </c>
       <c r="J26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2953,7 +2953,7 @@
         <v>10</v>
       </c>
       <c r="J27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2982,7 +2982,7 @@
         <v>10</v>
       </c>
       <c r="J28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -3011,7 +3011,7 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -3094,7 +3094,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3123,12 +3123,12 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B4" s="3">
         <v>5</v>
@@ -3143,16 +3143,16 @@
         <v>199</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="H4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="H4" t="s">
-        <v>159</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3181,7 +3181,7 @@
         <v>5</v>
       </c>
       <c r="J5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3210,7 +3210,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3239,7 +3239,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3268,7 +3268,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3297,7 +3297,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3326,7 +3326,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3355,7 +3355,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3384,7 +3384,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -3465,7 +3465,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3491,7 +3491,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3517,12 +3517,12 @@
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3534,16 +3534,16 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
+        <v>304</v>
+      </c>
+      <c r="H5" t="s">
+        <v>159</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
         <v>305</v>
-      </c>
-      <c r="H5" t="s">
-        <v>159</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3569,7 +3569,7 @@
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3595,7 +3595,7 @@
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3621,7 +3621,7 @@
         <v>0.1</v>
       </c>
       <c r="J8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3647,7 +3647,7 @@
         <v>0.01</v>
       </c>
       <c r="J9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3673,7 +3673,7 @@
         <v>0.5</v>
       </c>
       <c r="J10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3699,7 +3699,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3725,7 +3725,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3751,7 +3751,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -3777,7 +3777,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3803,7 +3803,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3832,7 +3832,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -3858,7 +3858,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -3884,7 +3884,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -3910,7 +3910,7 @@
         <v>0.01</v>
       </c>
       <c r="J19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3939,7 +3939,7 @@
         <v>0.01</v>
       </c>
       <c r="J20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -3965,7 +3965,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -3991,7 +3991,7 @@
         <v>0.5</v>
       </c>
       <c r="J22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -4020,7 +4020,7 @@
         <v>0.01</v>
       </c>
       <c r="J23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -4046,7 +4046,7 @@
         <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -4072,7 +4072,7 @@
         <v>5</v>
       </c>
       <c r="J25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -4084,7 +4084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49756CD-7B89-4299-B487-83FA9AC75873}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -4156,7 +4156,7 @@
         <v>0.01</v>
       </c>
       <c r="J2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4182,7 +4182,7 @@
         <v>1E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4208,7 +4208,7 @@
         <v>1E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -4234,7 +4234,7 @@
         <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -4260,7 +4260,7 @@
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4289,7 +4289,7 @@
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4315,7 +4315,7 @@
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4341,7 +4341,7 @@
         <v>0.01</v>
       </c>
       <c r="J9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4367,7 +4367,7 @@
         <v>0.01</v>
       </c>
       <c r="J10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4393,7 +4393,7 @@
         <v>0.01</v>
       </c>
       <c r="J11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -4477,7 +4477,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4506,7 +4506,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4535,7 +4535,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -4564,7 +4564,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -4593,7 +4593,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4622,7 +4622,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4651,7 +4651,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4680,7 +4680,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4709,7 +4709,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4738,7 +4738,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -4767,7 +4767,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -4796,7 +4796,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -4825,7 +4825,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -4854,7 +4854,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -4883,7 +4883,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -4912,7 +4912,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -4941,7 +4941,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -4970,7 +4970,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -4999,7 +4999,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -5028,7 +5028,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -5057,7 +5057,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -5086,7 +5086,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -5115,7 +5115,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -5144,7 +5144,7 @@
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -5173,7 +5173,7 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -5202,7 +5202,7 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -5231,7 +5231,7 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -5260,7 +5260,7 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -5289,7 +5289,7 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -5318,7 +5318,7 @@
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -5347,7 +5347,7 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -5376,7 +5376,7 @@
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
another minor update to expertise
</commit_message>
<xml_diff>
--- a/data/Apple_AF_Steinfurt_wRisk_30.xlsx
+++ b/data/Apple_AF_Steinfurt_wRisk_30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\UK_visa_docs\Apple\Apple_Agroforestry\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6390DAD1-1A4A-4AC1-830F-E3A7EB9E46C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9051DD43-8F45-471D-9AD2-643B0E8D8A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="2" r:id="rId1"/>
@@ -950,25 +950,25 @@
     <t>Data analyst;Market analyst</t>
   </si>
   <si>
-    <t>Data analyst;Agroforestry farmer;Market analyst;Policy-maker</t>
-  </si>
-  <si>
-    <t>Data analyst;Market analyst;Policy-maker;Agroforestry farmer</t>
-  </si>
-  <si>
-    <t>Data analyst;Agroforestry farmer</t>
-  </si>
-  <si>
-    <t>Agroforestry farmer;Data analyst;Policy-maker</t>
-  </si>
-  <si>
-    <t>Agroforestry farmer;Data analyst</t>
-  </si>
-  <si>
-    <t>Agroforestry farmer;Data analyst;Market analyst;Policy-maker</t>
-  </si>
-  <si>
-    <t>Agroforestry farmer;Policy-maker;Data analyst;Market analyst</t>
+    <t>Farmer;Policy-maker;Data analyst;Market analyst</t>
+  </si>
+  <si>
+    <t>Data analyst;Farmer;Market analyst;Policy-maker</t>
+  </si>
+  <si>
+    <t>Data analyst;Market analyst;Policy-maker;Farmer</t>
+  </si>
+  <si>
+    <t>Data analyst;Farmer</t>
+  </si>
+  <si>
+    <t>Farmer;Data analyst;Policy-maker</t>
+  </si>
+  <si>
+    <t>Farmer;Data analyst</t>
+  </si>
+  <si>
+    <t>Farmer;Data analyst;Market analyst;Policy-maker</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92018703-4177-49D8-B09E-62560F009CDF}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -1482,7 +1482,7 @@
         <v>1000</v>
       </c>
       <c r="J2" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1514,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1543,7 +1543,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1572,7 +1572,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1604,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -1616,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546B24F0-A477-4B95-8562-CC4F97744405}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1687,7 +1687,7 @@
         <v>0.1</v>
       </c>
       <c r="J2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1742,7 +1742,7 @@
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1797,7 +1797,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J6" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1826,7 +1826,7 @@
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1855,7 +1855,7 @@
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1913,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1942,7 +1942,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1971,7 +1971,7 @@
         <v>0.1</v>
       </c>
       <c r="J12" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2000,7 +2000,7 @@
         <v>100</v>
       </c>
       <c r="J13" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2029,7 +2029,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2087,7 +2087,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2116,7 +2116,7 @@
         <v>0.1</v>
       </c>
       <c r="J17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2145,7 +2145,7 @@
         <v>10</v>
       </c>
       <c r="J18" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -2228,7 +2228,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2257,7 +2257,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2286,7 +2286,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2315,7 +2315,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2344,7 +2344,7 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -2373,7 +2373,7 @@
         <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2431,7 +2431,7 @@
         <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2460,7 +2460,7 @@
         <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2489,7 +2489,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -2518,7 +2518,7 @@
         <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2547,7 +2547,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2576,7 +2576,7 @@
         <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2605,7 +2605,7 @@
         <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2634,7 +2634,7 @@
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2663,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2692,7 +2692,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2721,7 +2721,7 @@
         <v>10</v>
       </c>
       <c r="J19" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2750,7 +2750,7 @@
         <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2779,7 +2779,7 @@
         <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2808,7 +2808,7 @@
         <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -2837,7 +2837,7 @@
         <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -2866,7 +2866,7 @@
         <v>10</v>
       </c>
       <c r="J24" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2895,7 +2895,7 @@
         <v>10</v>
       </c>
       <c r="J25" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2924,7 +2924,7 @@
         <v>10</v>
       </c>
       <c r="J26" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2953,7 +2953,7 @@
         <v>10</v>
       </c>
       <c r="J27" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2982,7 +2982,7 @@
         <v>10</v>
       </c>
       <c r="J28" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -3011,7 +3011,7 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -3094,7 +3094,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3123,7 +3123,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3181,7 +3181,7 @@
         <v>5</v>
       </c>
       <c r="J5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3210,7 +3210,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3239,7 +3239,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3268,7 +3268,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3297,7 +3297,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3326,7 +3326,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3355,7 +3355,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3384,7 +3384,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -3465,7 +3465,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3491,7 +3491,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3517,7 +3517,7 @@
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3569,7 +3569,7 @@
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3595,7 +3595,7 @@
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3621,7 +3621,7 @@
         <v>0.1</v>
       </c>
       <c r="J8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3647,7 +3647,7 @@
         <v>0.01</v>
       </c>
       <c r="J9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3673,7 +3673,7 @@
         <v>0.5</v>
       </c>
       <c r="J10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3699,7 +3699,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3725,7 +3725,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3751,7 +3751,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -3777,7 +3777,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3803,7 +3803,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3832,7 +3832,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -3858,7 +3858,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -3884,7 +3884,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -3910,7 +3910,7 @@
         <v>0.01</v>
       </c>
       <c r="J19" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3939,7 +3939,7 @@
         <v>0.01</v>
       </c>
       <c r="J20" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -3965,7 +3965,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -3991,7 +3991,7 @@
         <v>0.5</v>
       </c>
       <c r="J22" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -4020,7 +4020,7 @@
         <v>0.01</v>
       </c>
       <c r="J23" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -4046,7 +4046,7 @@
         <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -4072,7 +4072,7 @@
         <v>5</v>
       </c>
       <c r="J25" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -4156,7 +4156,7 @@
         <v>0.01</v>
       </c>
       <c r="J2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4182,7 +4182,7 @@
         <v>1E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4208,7 +4208,7 @@
         <v>1E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -4234,7 +4234,7 @@
         <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -4260,7 +4260,7 @@
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4289,7 +4289,7 @@
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4315,7 +4315,7 @@
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4341,7 +4341,7 @@
         <v>0.01</v>
       </c>
       <c r="J9" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4367,7 +4367,7 @@
         <v>0.01</v>
       </c>
       <c r="J10" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4393,7 +4393,7 @@
         <v>0.01</v>
       </c>
       <c r="J11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>